<commit_message>
added json_comparator detector and reasoning check with failed-str{e}
</commit_message>
<xml_diff>
--- a/consolidated_report.xlsx
+++ b/consolidated_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,10 +471,15 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>giftcard_json_comparator</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Final Result</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Reason</t>
         </is>
@@ -493,7 +498,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -518,14 +523,15 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>giftcard_comparator=[Expected vs Observed Matched ?=NA]; giftcard_newrelic=[File_Name=ShipmentType_Null_No_Printer_831908000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=ShipmentType_Null_No_Printer_831908000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Mirakl Pushed to Fulfillment=No, Mirakl Refund Initiated=NA, Mirakl Refund Completed=NA]; mirakl_refund_newrelic=[File_Name=ShipmentType_Null_No_Printer_831908000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Refund Approved=No, Refund Payment Initiated=NA, Refund Completed=NA, Refund Notification Sent=No, Refund Error=NA]</t>
-        </is>
-      </c>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -540,7 +546,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -565,14 +571,15 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>giftcard_comparator=[Expected vs Observed Matched ?=NA]; giftcard_newrelic=[File_Name=Invalid_XML.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=Invalid_XML.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Mirakl Order Created=No, Mirakl Refund Initiated=No, Mirakl Refund Completed=NA]; mirakl_refund_newrelic=[File_Name=Invalid_XML.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Refund Request Received=No, Refund Payment Initiated=No, Refund Completed=NA, Refund Error=Validation failed]</t>
-        </is>
-      </c>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -587,7 +594,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -612,14 +619,15 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>giftcard_comparator=[Expected vs Observed Matched ?=NA]; giftcard_newrelic=[File_Name=REGULAR_GIFT_CARD with missing printer info_843597000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=REGULAR_GIFT_CARD with missing printer info_843597000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Mirakl Order Validated=No, Mirakl Refund Completed=No]; mirakl_refund_newrelic=[File_Name=REGULAR_GIFT_CARD with missing printer info_843597000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Refund Eligibility Checked=No, Refund Approved=No, Refund Completed=No, Refund Notification Sent=No, Refund Error=NA]</t>
-        </is>
-      </c>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -634,7 +642,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -659,14 +667,15 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>giftcard_comparator=[Expected vs Observed Matched ?=NA]; giftcard_newrelic=[File_Name=Kafka message with missing required fields_843595000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=Kafka message with missing required fields_843595000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Mirakl Order Created=No, Mirakl Order Validated=No, Mirakl Pushed to Fulfillment=No, Mirakl Refund Initiated=NA]; mirakl_refund_newrelic=[File_Name=Kafka message with missing required fields_843595000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Refund Payment Initiated=NA, Refund Error=Payment gateway timeout]</t>
-        </is>
-      </c>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -681,7 +690,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -706,14 +715,15 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>giftcard_comparator=[Expected vs Observed Matched ?=NA]; giftcard_newrelic=[File_Name=REGULAR_GIFT_CARD_843596000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=REGULAR_GIFT_CARD_843596000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Mirakl Pushed to Fulfillment=No, Mirakl Refund Initiated=No, Mirakl Refund Completed=No]; mirakl_refund_newrelic=[File_Name=REGULAR_GIFT_CARD_843596000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Refund Request Received=No, Refund Eligibility Checked=No, Refund Payment Initiated=No, Refund Completed=No, Refund Notification Sent=No, Refund Error=NA]</t>
-        </is>
-      </c>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -728,7 +738,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -758,7 +768,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>giftcard_comparator=[Expected vs Observed Matched ?=NA]; giftcard_newrelic=[File_Name=ShipmentType_Null_US_Printer_831909000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=ShipmentType_Null_US_Printer_831909000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Mirakl Pushed to Fulfillment=No, Mirakl Refund Initiated=NA, Mirakl Refund Completed=NA]; mirakl_refund_newrelic=[File_Name=ShipmentType_Null_US_Printer_831909000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Refund Approved=No, Refund Payment Initiated=NA, Refund Completed=NA, Refund Notification Sent=No, Refund Error=NA]</t>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>giftcard_json_comparator=[Reason=Field root['StyleHeaders'][0]['division'] exists in expected but missing in observed.; Field root['StyleHeaders'][0]['StyleDetails'][0]['division'] exists in expected but missing in observed.]</t>
         </is>
       </c>
     </row>
@@ -775,7 +790,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -805,7 +820,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>giftcard_comparator=[Expected vs Observed Matched ?=NA]; giftcard_newrelic=[File_Name=US_Printer_PRN11_831911000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=US_Printer_PRN11_831911000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Mirakl Order Created=No, Mirakl Refund Initiated=No, Mirakl Refund Completed=NA]; mirakl_refund_newrelic=[File_Name=US_Printer_PRN11_831911000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Refund Request Received=No, Refund Payment Initiated=No, Refund Completed=NA, Refund Error=Validation failed]</t>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>giftcard_json_comparator=[Reason=Field root['StyleHeaders'][0]['division'] exists in expected but missing in observed.; Field root['StyleHeaders'][0]['StyleDetails'][0]['division'] exists in expected but missing in observed.]</t>
         </is>
       </c>
     </row>
@@ -822,7 +842,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -852,7 +872,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>giftcard_newrelic=[File_Name=E_GIFT_CARD_845876577.xml, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=E_GIFT_CARD_845876577.xml, Mirakl Order Validated=No, Mirakl Refund Completed=No]; mirakl_refund_newrelic=[File_Name=E_GIFT_CARD_845876577.xml, Refund Eligibility Checked=No, Refund Approved=No, Refund Completed=No, Refund Notification Sent=No, Refund Error=NA]</t>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>giftcard_json_comparator=[Reason=Field root['StyleHeaders'][0]['division'] exists in expected but missing in observed.; Field root['StyleHeaders'][0]['StyleDetails'][0]['division'] exists in expected but missing in observed.]</t>
         </is>
       </c>
     </row>
@@ -869,7 +894,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -899,7 +924,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>giftcard_comparator=[Expected vs Observed Matched ?=NA]; giftcard_newrelic=[File_Name=ShipmentNo-is extract E_GIFT_CARD.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=ShipmentNo-is extract E_GIFT_CARD.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Mirakl Order Created=No, Mirakl Order Validated=No, Mirakl Pushed to Fulfillment=No, Mirakl Refund Initiated=NA]; mirakl_refund_newrelic=[File_Name=ShipmentNo-is extract E_GIFT_CARD.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Refund Payment Initiated=NA, Refund Error=Payment gateway timeout]</t>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>giftcard_json_comparator=[Reason=Field root['StyleHeaders'][0]['division'] exists in expected but missing in observed.; Field root['StyleHeaders'][0]['StyleDetails'][0]['division'] exists in expected but missing in observed.]</t>
         </is>
       </c>
     </row>
@@ -916,7 +946,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -946,7 +976,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>giftcard_newrelic=[File_Name=E_GIFT_CARD_843593000.xml, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=E_GIFT_CARD_843593000.xml, Mirakl Pushed to Fulfillment=No, Mirakl Refund Initiated=No, Mirakl Refund Completed=No]; mirakl_refund_newrelic=[File_Name=E_GIFT_CARD_843593000.xml, Refund Request Received=No, Refund Eligibility Checked=No, Refund Payment Initiated=No, Refund Completed=No, Refund Notification Sent=No, Refund Error=NA]</t>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>giftcard_json_comparator=[Reason=Field root['StyleHeaders'][0]['division'] exists in expected but missing in observed.; Field root['StyleHeaders'][0]['StyleDetails'][0]['division'] exists in expected but missing in observed.]</t>
         </is>
       </c>
     </row>
@@ -963,7 +998,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -988,14 +1023,15 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>giftcard_newrelic=[File_Name=E_GIFT_CARD_REFUND_843594000.xml, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=E_GIFT_CARD_REFUND_843594000.xml, Mirakl Pushed to Fulfillment=No, Mirakl Refund Initiated=NA, Mirakl Refund Completed=NA]; mirakl_refund_newrelic=[File_Name=E_GIFT_CARD_REFUND_843594000.xml, Refund Approved=No, Refund Payment Initiated=NA, Refund Completed=NA, Refund Notification Sent=No, Refund Error=NA]</t>
-        </is>
-      </c>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1010,7 +1046,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1035,14 +1071,15 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>giftcard_comparator=[Expected vs Observed Matched ?=NA]; giftcard_newrelic=[File_Name=UK_Printer_UKPFGIF01_831910000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Started processing the transaction=No, Received message from Sterling=No, GiftCardPrint XML=No, GiftCardPrint message processed successfully to email_subscribe=No, Sending GiftCardPrint message to Kafka topic=No, Completed processing the transaction=No, send_message_to_printer=No, Sending Label message to printer=No, Response from printer:=No, Label message processed successfully=No, Error occurred during GiftCardPrint transformation=No, Error processing the message=No]; mirakl_order_newrelic=[File_Name=UK_Printer_UKPFGIF01_831910000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Mirakl Order Created=No, Mirakl Refund Initiated=No, Mirakl Refund Completed=NA]; mirakl_refund_newrelic=[File_Name=UK_Printer_UKPFGIF01_831910000.xml, Applicable_For_Consumer_Topic ?=No, Posted_To_Consumer_Topic ?=No, Expected vs Observed Matched ?=NA, Refund Request Received=No, Refund Payment Initiated=No, Refund Completed=NA, Refund Error=Validation failed]</t>
-        </is>
-      </c>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>